<commit_message>
ExcelUO - some more progress
Added capabilities for 4 streams @ input and output.
Initial design for UIEditor

Further work needed prior to release.
</commit_message>
<xml_diff>
--- a/DWSIM/bin/x86/Release/TemplateExcelUO.xlsx
+++ b/DWSIM/bin/x86/Release/TemplateExcelUO.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="14115" windowHeight="4170"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
   <si>
     <t>Input streams to Unit</t>
   </si>
@@ -45,10 +45,19 @@
     <t>[mol/s]</t>
   </si>
   <si>
-    <t>[Kg/s]</t>
-  </si>
-  <si>
     <t>Output streams from Unit</t>
+  </si>
+  <si>
+    <t>Stream 2</t>
+  </si>
+  <si>
+    <t>Stream 3</t>
+  </si>
+  <si>
+    <t>Stream 4</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -114,10 +123,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -419,62 +428,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <sheetPr codeName="Tabelle1"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="17" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="18" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="19" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="20" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="22" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -482,10 +538,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <sheetPr codeName="Tabelle2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -493,55 +550,79 @@
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2">
-        <f>Input!B6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
-        <f>Input!B7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
-        <f>Input!B8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -551,6 +632,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>